<commit_message>
- Added the report - Minor fixes in the Gantt Chart
</commit_message>
<xml_diff>
--- a/2017-10-1_project-methodology_ca1_Mathias-Nervik_fp.xlsx
+++ b/2017-10-1_project-methodology_ca1_Mathias-Nervik_fp.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Y:\Project Methodology\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nervi\Documents\Lofthus-frukt-og-saft\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -193,7 +193,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -203,6 +203,13 @@
     </font>
     <font>
       <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -295,61 +302,62 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -678,58 +686,64 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DD9A3F53-14B8-4867-8BA3-1EBF8EB96D2D}">
   <dimension ref="A1:AK30"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="C30" sqref="C30"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="I30" sqref="I30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="22.140625" customWidth="1"/>
-    <col min="2" max="2" width="10.140625" customWidth="1"/>
-    <col min="3" max="3" width="33.42578125" customWidth="1"/>
-    <col min="4" max="4" width="19" customWidth="1"/>
-    <col min="5" max="5" width="18" customWidth="1"/>
-    <col min="7" max="7" width="14.42578125" customWidth="1"/>
-    <col min="9" max="9" width="16" customWidth="1"/>
-    <col min="15" max="15" width="13.28515625" customWidth="1"/>
-    <col min="17" max="17" width="13.5703125" customWidth="1"/>
-    <col min="21" max="21" width="17" customWidth="1"/>
-    <col min="22" max="22" width="17.5703125" customWidth="1"/>
-    <col min="23" max="23" width="17.28515625" customWidth="1"/>
-    <col min="24" max="24" width="13.42578125" customWidth="1"/>
-    <col min="25" max="25" width="9.85546875" customWidth="1"/>
+    <col min="1" max="1" width="25.7109375" style="1" customWidth="1"/>
+    <col min="2" max="2" width="10.140625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="33.42578125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="19" style="1" customWidth="1"/>
+    <col min="5" max="5" width="18" style="1" customWidth="1"/>
+    <col min="6" max="6" width="11.42578125" style="1"/>
+    <col min="7" max="7" width="16.5703125" style="1" customWidth="1"/>
+    <col min="8" max="8" width="11.42578125" style="1"/>
+    <col min="9" max="9" width="16" style="1" customWidth="1"/>
+    <col min="10" max="14" width="11.42578125" style="1"/>
+    <col min="15" max="15" width="16.140625" style="1" customWidth="1"/>
+    <col min="16" max="16" width="11.42578125" style="1"/>
+    <col min="17" max="17" width="19.140625" style="1" customWidth="1"/>
+    <col min="18" max="20" width="11.42578125" style="1"/>
+    <col min="21" max="21" width="15.140625" style="1" customWidth="1"/>
+    <col min="22" max="22" width="27.140625" style="1" customWidth="1"/>
+    <col min="23" max="23" width="17.28515625" style="1" customWidth="1"/>
+    <col min="24" max="24" width="16.28515625" style="1" customWidth="1"/>
+    <col min="25" max="25" width="12.7109375" style="1" customWidth="1"/>
+    <col min="26" max="16384" width="11.42578125" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:37" ht="10.5" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="2" spans="1:37" ht="54.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C2" s="18" t="s">
+      <c r="C2" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="D2" s="18"/>
-      <c r="E2" s="18"/>
-      <c r="F2" s="18"/>
-      <c r="G2" s="18"/>
-      <c r="I2" s="17" t="s">
+      <c r="D2" s="2"/>
+      <c r="E2" s="2"/>
+      <c r="F2" s="2"/>
+      <c r="G2" s="2"/>
+      <c r="I2" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="J2" s="17"/>
-      <c r="K2" s="17"/>
-      <c r="L2" s="17"/>
-      <c r="M2" s="17"/>
-      <c r="O2" s="16" t="s">
+      <c r="J2" s="3"/>
+      <c r="K2" s="3"/>
+      <c r="L2" s="3"/>
+      <c r="M2" s="3"/>
+      <c r="O2" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="P2" s="16"/>
-      <c r="Q2" s="16"/>
-      <c r="R2" s="16"/>
-      <c r="S2" s="16"/>
-      <c r="U2" s="15" t="s">
+      <c r="P2" s="4"/>
+      <c r="Q2" s="4"/>
+      <c r="R2" s="4"/>
+      <c r="S2" s="4"/>
+      <c r="U2" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="V2" s="15"/>
-      <c r="W2" s="15"/>
-      <c r="X2" s="15"/>
-      <c r="Y2" s="15"/>
+      <c r="V2" s="5"/>
+      <c r="W2" s="5"/>
+      <c r="X2" s="5"/>
+      <c r="Y2" s="5"/>
     </row>
     <row r="3" spans="1:37" ht="8.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="4" spans="1:37" x14ac:dyDescent="0.25">
@@ -748,258 +762,258 @@
       <c r="G4" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="I4" s="3" t="s">
+      <c r="I4" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="J4" s="3" t="s">
+      <c r="J4" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="K4" s="3" t="s">
+      <c r="K4" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="L4" s="3" t="s">
+      <c r="L4" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="M4" s="3" t="s">
+      <c r="M4" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="O4" s="2" t="s">
+      <c r="O4" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="P4" s="2" t="s">
+      <c r="P4" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="Q4" s="2" t="s">
+      <c r="Q4" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="R4" s="2" t="s">
+      <c r="R4" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="S4" s="2" t="s">
+      <c r="S4" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="U4" s="1" t="s">
+      <c r="U4" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="V4" s="1" t="s">
+      <c r="V4" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="W4" s="1" t="s">
+      <c r="W4" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="X4" s="1" t="s">
+      <c r="X4" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="Y4" s="1" t="s">
+      <c r="Y4" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="Z4" s="4"/>
-      <c r="AA4" s="4"/>
-      <c r="AB4" s="4"/>
-      <c r="AC4" s="4"/>
-      <c r="AD4" s="4"/>
-      <c r="AE4" s="4"/>
-      <c r="AF4" s="4"/>
-      <c r="AG4" s="4"/>
-      <c r="AH4" s="4"/>
-      <c r="AI4" s="4"/>
-      <c r="AJ4" s="4"/>
-      <c r="AK4" s="4"/>
+      <c r="Z4" s="10"/>
+      <c r="AA4" s="10"/>
+      <c r="AB4" s="10"/>
+      <c r="AC4" s="10"/>
+      <c r="AD4" s="10"/>
+      <c r="AE4" s="10"/>
+      <c r="AF4" s="10"/>
+      <c r="AG4" s="10"/>
+      <c r="AH4" s="10"/>
+      <c r="AI4" s="10"/>
+      <c r="AJ4" s="10"/>
+      <c r="AK4" s="10"/>
     </row>
     <row r="5" spans="1:37" ht="6" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="6" spans="1:37" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="12" t="s">
+      <c r="A6" s="11" t="s">
         <v>39</v>
       </c>
-      <c r="C6" s="10" t="s">
+      <c r="C6" s="12" t="s">
         <v>49</v>
       </c>
-      <c r="D6" s="10"/>
-      <c r="E6" s="10"/>
-      <c r="F6" s="10"/>
-      <c r="G6" s="10"/>
-      <c r="I6" s="10" t="s">
+      <c r="D6" s="12"/>
+      <c r="E6" s="12"/>
+      <c r="F6" s="12"/>
+      <c r="G6" s="12"/>
+      <c r="I6" s="12" t="s">
         <v>32</v>
       </c>
-      <c r="J6" s="10"/>
-      <c r="K6" s="10"/>
-      <c r="L6" s="10"/>
-      <c r="M6" s="10"/>
-      <c r="O6" s="10" t="s">
+      <c r="J6" s="12"/>
+      <c r="K6" s="12"/>
+      <c r="L6" s="12"/>
+      <c r="M6" s="12"/>
+      <c r="O6" s="12" t="s">
         <v>32</v>
       </c>
-      <c r="P6" s="10"/>
-      <c r="Q6" s="10"/>
-      <c r="R6" s="10"/>
-      <c r="S6" s="10"/>
-      <c r="U6" s="10" t="s">
+      <c r="P6" s="12"/>
+      <c r="Q6" s="12"/>
+      <c r="R6" s="12"/>
+      <c r="S6" s="12"/>
+      <c r="U6" s="12" t="s">
         <v>32</v>
       </c>
-      <c r="V6" s="10"/>
-      <c r="W6" s="10"/>
-      <c r="X6" s="10"/>
-      <c r="Y6" s="10"/>
+      <c r="V6" s="12"/>
+      <c r="W6" s="12"/>
+      <c r="X6" s="12"/>
+      <c r="Y6" s="12"/>
     </row>
     <row r="7" spans="1:37" ht="6" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="8" spans="1:37" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="14" t="s">
+      <c r="A8" s="13" t="s">
         <v>40</v>
       </c>
-      <c r="C8" s="7" t="s">
+      <c r="C8" s="14" t="s">
         <v>20</v>
       </c>
-      <c r="D8" s="5"/>
+      <c r="D8" s="15"/>
     </row>
     <row r="9" spans="1:37" ht="3.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="10" spans="1:37" ht="48.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="14" t="s">
+      <c r="A10" s="13" t="s">
         <v>41</v>
       </c>
-      <c r="B10" s="19"/>
-      <c r="C10" s="8" t="s">
+      <c r="B10" s="16"/>
+      <c r="C10" s="17" t="s">
         <v>21</v>
       </c>
-      <c r="D10" s="8"/>
+      <c r="D10" s="17"/>
     </row>
     <row r="11" spans="1:37" ht="6" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="12" spans="1:37" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="12" t="s">
+      <c r="A12" s="11" t="s">
         <v>42</v>
       </c>
-      <c r="E12" s="8" t="s">
+      <c r="E12" s="17" t="s">
         <v>22</v>
       </c>
-      <c r="F12" s="8"/>
-      <c r="G12" s="8"/>
+      <c r="F12" s="17"/>
+      <c r="G12" s="17"/>
     </row>
     <row r="13" spans="1:37" ht="7.5" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="14" spans="1:37" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="13" t="s">
+      <c r="A14" s="18" t="s">
         <v>44</v>
       </c>
-      <c r="G14" s="9" t="s">
+      <c r="G14" s="19" t="s">
         <v>23</v>
       </c>
-      <c r="I14" s="10" t="s">
+      <c r="I14" s="12" t="s">
         <v>24</v>
       </c>
-      <c r="J14" s="10"/>
+      <c r="J14" s="12"/>
     </row>
     <row r="15" spans="1:37" ht="5.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="16" spans="1:37" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="11" t="s">
+      <c r="A16" s="20" t="s">
         <v>45</v>
       </c>
-      <c r="K16" s="10" t="s">
+      <c r="K16" s="12" t="s">
         <v>25</v>
       </c>
-      <c r="L16" s="10"/>
-      <c r="M16" s="10"/>
-      <c r="O16" s="9" t="s">
+      <c r="L16" s="12"/>
+      <c r="M16" s="12"/>
+      <c r="O16" s="19" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="17" spans="1:25" ht="6.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="18" spans="1:25" ht="30" x14ac:dyDescent="0.25">
-      <c r="A18" s="14" t="s">
+      <c r="A18" s="13" t="s">
         <v>46</v>
       </c>
-      <c r="K18" s="8" t="s">
+      <c r="K18" s="17" t="s">
         <v>26</v>
       </c>
-      <c r="L18" s="8"/>
-      <c r="M18" s="8"/>
+      <c r="L18" s="17"/>
+      <c r="M18" s="17"/>
     </row>
     <row r="19" spans="1:25" ht="6" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="20" spans="1:25" ht="30" x14ac:dyDescent="0.25">
-      <c r="A20" s="14" t="s">
+      <c r="A20" s="13" t="s">
         <v>43</v>
       </c>
-      <c r="P20" s="10" t="s">
+      <c r="P20" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="Q20" s="10"/>
-      <c r="U20" s="9" t="s">
+      <c r="Q20" s="12"/>
+      <c r="U20" s="19" t="s">
         <v>35</v>
       </c>
-      <c r="V20" s="5"/>
+      <c r="V20" s="15"/>
     </row>
     <row r="21" spans="1:25" ht="6.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="22" spans="1:25" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="12" t="s">
+      <c r="A22" s="11" t="s">
         <v>47</v>
       </c>
-      <c r="O22" s="10" t="s">
+      <c r="O22" s="12" t="s">
         <v>34</v>
       </c>
-      <c r="P22" s="10"/>
-      <c r="Q22" s="10"/>
-      <c r="R22" s="10"/>
-      <c r="S22" s="10"/>
-      <c r="U22" s="10" t="s">
+      <c r="P22" s="12"/>
+      <c r="Q22" s="12"/>
+      <c r="R22" s="12"/>
+      <c r="S22" s="12"/>
+      <c r="U22" s="12" t="s">
         <v>34</v>
       </c>
-      <c r="V22" s="10"/>
-      <c r="W22" s="5"/>
-      <c r="X22" s="5"/>
-      <c r="Y22" s="5"/>
+      <c r="V22" s="12"/>
+      <c r="W22" s="15"/>
+      <c r="X22" s="15"/>
+      <c r="Y22" s="15"/>
     </row>
     <row r="23" spans="1:25" ht="6.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="24" spans="1:25" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="12" t="s">
+      <c r="A24" s="11" t="s">
         <v>47</v>
       </c>
-      <c r="V24" s="10" t="s">
+      <c r="V24" s="12" t="s">
         <v>36</v>
       </c>
-      <c r="W24" s="10"/>
+      <c r="W24" s="12"/>
     </row>
     <row r="25" spans="1:25" ht="7.5" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="26" spans="1:25" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="12" t="s">
+      <c r="A26" s="11" t="s">
         <v>47</v>
       </c>
-      <c r="W26" s="9" t="s">
+      <c r="W26" s="19" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="27" spans="1:25" ht="5.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="28" spans="1:25" ht="45" x14ac:dyDescent="0.25">
-      <c r="A28" s="14" t="s">
+      <c r="A28" s="13" t="s">
         <v>44</v>
       </c>
-      <c r="X28" s="9" t="s">
+      <c r="X28" s="19" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="29" spans="1:25" ht="6.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="30" spans="1:25" ht="60" x14ac:dyDescent="0.25">
-      <c r="A30" s="14" t="s">
+    <row r="30" spans="1:25" ht="65.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="13" t="s">
         <v>48</v>
       </c>
-      <c r="Y30" s="9" t="s">
+      <c r="Y30" s="19" t="s">
         <v>30</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="17">
-    <mergeCell ref="K18:M18"/>
-    <mergeCell ref="I14:J14"/>
-    <mergeCell ref="K16:M16"/>
-    <mergeCell ref="C2:G2"/>
-    <mergeCell ref="I2:M2"/>
+    <mergeCell ref="P20:Q20"/>
+    <mergeCell ref="O22:S22"/>
+    <mergeCell ref="U22:V22"/>
+    <mergeCell ref="V24:W24"/>
+    <mergeCell ref="C10:D10"/>
+    <mergeCell ref="E12:G12"/>
     <mergeCell ref="U2:Y2"/>
     <mergeCell ref="O2:S2"/>
     <mergeCell ref="C6:G6"/>
     <mergeCell ref="I6:M6"/>
     <mergeCell ref="O6:S6"/>
     <mergeCell ref="U6:Y6"/>
-    <mergeCell ref="P20:Q20"/>
-    <mergeCell ref="O22:S22"/>
-    <mergeCell ref="U22:V22"/>
-    <mergeCell ref="V24:W24"/>
-    <mergeCell ref="C10:D10"/>
-    <mergeCell ref="E12:G12"/>
+    <mergeCell ref="K18:M18"/>
+    <mergeCell ref="I14:J14"/>
+    <mergeCell ref="K16:M16"/>
+    <mergeCell ref="C2:G2"/>
+    <mergeCell ref="I2:M2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>